<commit_message>
updated gmm gmm_sector_avg and economic data files
</commit_message>
<xml_diff>
--- a/Data/Economic_Data.xlsx
+++ b/Data/Economic_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28230"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\G-DRIVE 21-07-22\Dr Afaq Qazi\Fouzia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maryum Butt\Desktop\NRPU\Backend 28-4-2025\NRPU-Backend\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{06851585-FB0F-42CB-976C-8F467048D54F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7CB06398-180A-4384-B784-5FF9412D9409}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{860C2C07-40C3-4EFF-B0C6-F4B2E2798D15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{56162159-60BA-4D87-81E4-247349A9A007}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{56162159-60BA-4D87-81E4-247349A9A007}"/>
   </bookViews>
   <sheets>
     <sheet name="Complete Data" sheetId="1" r:id="rId1"/>
@@ -111,7 +111,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -209,7 +209,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -232,6 +232,16 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -547,33 +557,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79EC7623-B4A2-41C4-820D-6C294FDFEE88}">
-  <dimension ref="A1:T23"/>
+  <dimension ref="A1:T24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.81640625" customWidth="1"/>
+    <col min="4" max="4" width="11.7265625" customWidth="1"/>
     <col min="5" max="5" width="33" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.7265625" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" customWidth="1"/>
-    <col min="9" max="10" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.453125" customWidth="1"/>
+    <col min="9" max="10" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.7265625" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="16.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -603,7 +613,7 @@
       <c r="S1" s="6"/>
       <c r="T1" s="6"/>
     </row>
-    <row r="2" spans="1:20" s="1" customFormat="1" ht="128.25" customHeight="1">
+    <row r="2" spans="1:20" s="1" customFormat="1" ht="128.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8"/>
       <c r="B2" s="2" t="s">
         <v>4</v>
@@ -663,7 +673,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>2002</v>
       </c>
@@ -721,7 +731,7 @@
         <v>101.623106200159</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>2003</v>
       </c>
@@ -779,7 +789,7 @@
         <v>98.841617635701397</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>2004</v>
       </c>
@@ -839,7 +849,7 @@
         <v>98.022364672626907</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>2005</v>
       </c>
@@ -901,7 +911,7 @@
         <v>100.976952429327</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>2006</v>
       </c>
@@ -961,7 +971,7 @@
         <v>103.785897514616</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>2007</v>
       </c>
@@ -1023,7 +1033,7 @@
         <v>102.327991278422</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>2008</v>
       </c>
@@ -1083,7 +1093,7 @@
         <v>97.385477164951496</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>2009</v>
       </c>
@@ -1143,7 +1153,7 @@
         <v>96.486922934314194</v>
       </c>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>2010</v>
       </c>
@@ -1205,7 +1215,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>2011</v>
       </c>
@@ -1267,7 +1277,7 @@
         <v>102.42303358976901</v>
       </c>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>2012</v>
       </c>
@@ -1327,7 +1337,7 @@
         <v>103.79738787321401</v>
       </c>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>2013</v>
       </c>
@@ -1389,7 +1399,7 @@
         <v>100.882152343794</v>
       </c>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>2014</v>
       </c>
@@ -1449,7 +1459,7 @@
         <v>107.81697846807</v>
       </c>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>2015</v>
       </c>
@@ -1511,7 +1521,7 @@
         <v>116.008543769516</v>
       </c>
     </row>
-    <row r="17" spans="1:20">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>2016</v>
       </c>
@@ -1571,7 +1581,7 @@
         <v>119.66888182492499</v>
       </c>
     </row>
-    <row r="18" spans="1:20">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>2017</v>
       </c>
@@ -1629,7 +1639,7 @@
         <v>121.650040240667</v>
       </c>
     </row>
-    <row r="19" spans="1:20">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>2018</v>
       </c>
@@ -1691,7 +1701,7 @@
         <v>107.266223978106</v>
       </c>
     </row>
-    <row r="20" spans="1:20">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>2019</v>
       </c>
@@ -1751,7 +1761,7 @@
         <v>97.260650578097099</v>
       </c>
     </row>
-    <row r="21" spans="1:20">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
         <v>2020</v>
       </c>
@@ -1809,7 +1819,7 @@
         <v>97.5741386674312</v>
       </c>
     </row>
-    <row r="22" spans="1:20">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
         <v>2021</v>
       </c>
@@ -1869,7 +1879,7 @@
         <v>100.257460718608</v>
       </c>
     </row>
-    <row r="23" spans="1:20">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A23" s="3">
         <v>2022</v>
       </c>
@@ -1925,6 +1935,66 @@
       </c>
       <c r="T23" s="4">
         <v>97.001532283817696</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A24" s="12">
+        <v>2023</v>
+      </c>
+      <c r="B24" s="9">
+        <v>-0.57999999999999996</v>
+      </c>
+      <c r="C24" s="9">
+        <v>-1.93</v>
+      </c>
+      <c r="D24" s="9">
+        <v>-0.99</v>
+      </c>
+      <c r="E24" s="9">
+        <v>3</v>
+      </c>
+      <c r="F24" s="9">
+        <v>-0.86</v>
+      </c>
+      <c r="G24" s="11"/>
+      <c r="H24" s="9">
+        <v>5.4080000000000004</v>
+      </c>
+      <c r="I24" s="9">
+        <v>1616.3068878659999</v>
+      </c>
+      <c r="J24" s="9">
+        <v>1365.2774322242999</v>
+      </c>
+      <c r="K24" s="9">
+        <v>-3.96925228069165E-2</v>
+      </c>
+      <c r="L24" s="10">
+        <v>40953671000000</v>
+      </c>
+      <c r="M24" s="9">
+        <v>30.768128065700498</v>
+      </c>
+      <c r="N24" s="9">
+        <v>-0.24421476876381301</v>
+      </c>
+      <c r="O24" s="9">
+        <v>-825231745.482939</v>
+      </c>
+      <c r="P24" s="9">
+        <v>43.260843757783597</v>
+      </c>
+      <c r="Q24" s="9">
+        <v>42.571738430231598</v>
+      </c>
+      <c r="R24" s="9">
+        <v>16.253063175299999</v>
+      </c>
+      <c r="S24" s="9">
+        <v>280.35611165514001</v>
+      </c>
+      <c r="T24" s="9">
+        <v>91.394551203056807</v>
       </c>
     </row>
   </sheetData>

</xml_diff>